<commit_message>
Updates docentry spreadsheet with new data
Refreshes spreadsheet contents to ensure alignment with
latest requirements or source data. Improves accuracy for
related processes or documentation.
</commit_message>
<xml_diff>
--- a/patchApiSma/docentry.xlsx
+++ b/patchApiSma/docentry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\scripts\patchApiSma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F4CBCB-04D5-4EAA-9CAF-12D12D2CD0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FC9D94-1E1D-41B5-A07C-82D10D80B686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26635121-3474-4A8D-AE0F-C22F0D8F450D}"/>
   </bookViews>
@@ -427,22 +427,22 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>70521</v>
+        <v>70713</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>70622</v>
+        <v>70716</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>70632</v>
+        <v>70718</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>70640</v>
+        <v>70720</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Agregar manejo de carga y actualización individual de tarjetas en el dashboard
</commit_message>
<xml_diff>
--- a/patchApiSma/docentry.xlsx
+++ b/patchApiSma/docentry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\scripts\patchApiSma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FC9D94-1E1D-41B5-A07C-82D10D80B686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F309F2-CFB0-4746-AC17-DCE0A6FD5DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26635121-3474-4A8D-AE0F-C22F0D8F450D}"/>
   </bookViews>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1922D5-C29D-42F9-909F-8E809F7BE4E8}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,22 +427,37 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>70713</v>
+        <v>70960</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>70716</v>
+        <v>71021</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>70718</v>
+        <v>71031</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>70720</v>
+        <v>71037</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>71038</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>71057</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>71084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Actualizar el archivo docentry.xlsx con nuevos datos
</commit_message>
<xml_diff>
--- a/patchApiSma/docentry.xlsx
+++ b/patchApiSma/docentry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\scripts\patchApiSma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F309F2-CFB0-4746-AC17-DCE0A6FD5DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAB1FBD-80D3-419E-A11B-6618FE77EA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26635121-3474-4A8D-AE0F-C22F0D8F450D}"/>
   </bookViews>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1922D5-C29D-42F9-909F-8E809F7BE4E8}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,37 +427,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>70960</v>
+        <v>71362</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>71021</v>
+        <v>71405</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>71031</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>71037</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>71038</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>71057</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>71084</v>
+        <v>71409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: actualizar el archivo docentry.xlsx con cambios binarios
</commit_message>
<xml_diff>
--- a/patchApiSma/docentry.xlsx
+++ b/patchApiSma/docentry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\scripts\patchApiSma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAB1FBD-80D3-419E-A11B-6618FE77EA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D01774E-5D91-407F-BB9F-6120AC62A884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26635121-3474-4A8D-AE0F-C22F0D8F450D}"/>
   </bookViews>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1922D5-C29D-42F9-909F-8E809F7BE4E8}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,17 +427,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>71362</v>
+        <v>71472</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>71405</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>71409</v>
+        <v>71475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: actualizar archivos binarios y agregar nuevos registros de errores en errores.txt
</commit_message>
<xml_diff>
--- a/patchApiSma/docentry.xlsx
+++ b/patchApiSma/docentry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\scripts\patchApiSma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D01774E-5D91-407F-BB9F-6120AC62A884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCDFBBB-1ECA-48FA-B6F2-BEECE74F2372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26635121-3474-4A8D-AE0F-C22F0D8F450D}"/>
   </bookViews>
@@ -95,9 +95,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1922D5-C29D-42F9-909F-8E809F7BE4E8}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,13 +429,8 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>71472</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>71475</v>
+      <c r="A2" s="2">
+        <v>138158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: agregar script para sincronización masiva de órdenes desde Excel
</commit_message>
<xml_diff>
--- a/patchApiSma/docentry.xlsx
+++ b/patchApiSma/docentry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\scripts\patchApiSma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547021A8-C0D3-4D34-A05D-8E3965B5D70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9D8957-359C-4365-8DAD-C5C6928B4AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26635121-3474-4A8D-AE0F-C22F0D8F450D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26635121-3474-4A8D-AE0F-C22F0D8F450D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,16 +34,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>DocEntry</t>
+  </si>
+  <si>
+    <t>2025-9539-23APR-3</t>
+  </si>
+  <si>
+    <t>2025-121390</t>
+  </si>
+  <si>
+    <t>2025-121388</t>
+  </si>
+  <si>
+    <t>2025-121735</t>
+  </si>
+  <si>
+    <t>2025-121735-A1</t>
+  </si>
+  <si>
+    <t>2025-122352</t>
+  </si>
+  <si>
+    <t>2025-122352-A2</t>
+  </si>
+  <si>
+    <t>2025-10347-20JUN-2</t>
+  </si>
+  <si>
+    <t>2025-10347-20JUN-3</t>
+  </si>
+  <si>
+    <t>2025-123533</t>
+  </si>
+  <si>
+    <t>REQ-13</t>
+  </si>
+  <si>
+    <t>2025-10582-19JUL-1</t>
+  </si>
+  <si>
+    <t>2025-124983</t>
+  </si>
+  <si>
+    <t>2025-128558</t>
+  </si>
+  <si>
+    <t>2025-128547</t>
+  </si>
+  <si>
+    <t>2025-128536</t>
+  </si>
+  <si>
+    <t>2025-128584</t>
+  </si>
+  <si>
+    <t>2025-11704-20OCT-1</t>
+  </si>
+  <si>
+    <t>2025-129624</t>
+  </si>
+  <si>
+    <t>2025-129986-A1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,30 +111,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -82,23 +128,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,13 +448,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1922D5-C29D-42F9-909F-8E809F7BE4E8}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -427,83 +465,103 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>70082</v>
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>73300</v>
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>73301</v>
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>73303</v>
+      <c r="A5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>73304</v>
+      <c r="A6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>73306</v>
+      <c r="A7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>73361</v>
+      <c r="A8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>73362</v>
+      <c r="A9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>73373</v>
+      <c r="A10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>73375</v>
+      <c r="A11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>73377</v>
+      <c r="A12" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>73378</v>
+      <c r="A13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>73421</v>
+      <c r="A14" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>73436</v>
+      <c r="A15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>73449</v>
+      <c r="A16" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>73459</v>
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: actualizar archivo Excel docentry.xlsx
</commit_message>
<xml_diff>
--- a/patchApiSma/docentry.xlsx
+++ b/patchApiSma/docentry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\scripts\patchApiSma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9D8957-359C-4365-8DAD-C5C6928B4AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D6EEED-A14E-4DC0-AE2D-AFFC761290FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26635121-3474-4A8D-AE0F-C22F0D8F450D}"/>
   </bookViews>
@@ -34,69 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>DocEntry</t>
-  </si>
-  <si>
-    <t>2025-9539-23APR-3</t>
-  </si>
-  <si>
-    <t>2025-121390</t>
-  </si>
-  <si>
-    <t>2025-121388</t>
-  </si>
-  <si>
-    <t>2025-121735</t>
-  </si>
-  <si>
-    <t>2025-121735-A1</t>
-  </si>
-  <si>
-    <t>2025-122352</t>
-  </si>
-  <si>
-    <t>2025-122352-A2</t>
-  </si>
-  <si>
-    <t>2025-10347-20JUN-2</t>
-  </si>
-  <si>
-    <t>2025-10347-20JUN-3</t>
-  </si>
-  <si>
-    <t>2025-123533</t>
-  </si>
-  <si>
-    <t>REQ-13</t>
-  </si>
-  <si>
-    <t>2025-10582-19JUL-1</t>
-  </si>
-  <si>
-    <t>2025-124983</t>
-  </si>
-  <si>
-    <t>2025-128558</t>
-  </si>
-  <si>
-    <t>2025-128547</t>
-  </si>
-  <si>
-    <t>2025-128536</t>
-  </si>
-  <si>
-    <t>2025-128584</t>
-  </si>
-  <si>
-    <t>2025-11704-20OCT-1</t>
-  </si>
-  <si>
-    <t>2025-129624</t>
-  </si>
-  <si>
-    <t>2025-129986-A1</t>
   </si>
 </sst>
 </file>
@@ -448,15 +388,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1922D5-C29D-42F9-909F-8E809F7BE4E8}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -465,103 +405,58 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2">
+        <v>73749</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
+      <c r="A3">
+        <v>73753</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="A4">
+        <v>73763</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
+      <c r="A5">
+        <v>73764</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
+      <c r="A6">
+        <v>73771</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
+      <c r="A7">
+        <v>73801</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
+      <c r="A8">
+        <v>73682</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
+      <c r="A9">
+        <v>73688</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
+      <c r="A10">
+        <v>73698</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
+      <c r="A11">
+        <v>73699</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
+      <c r="A12">
+        <v>73733</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: agregar script para actualizar DocEntries desde Excel
</commit_message>
<xml_diff>
--- a/patchApiSma/docentry.xlsx
+++ b/patchApiSma/docentry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\scripts\patchApiSma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D6EEED-A14E-4DC0-AE2D-AFFC761290FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCCD284-9DFE-4EBD-BC84-2115DAEB57F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26635121-3474-4A8D-AE0F-C22F0D8F450D}"/>
   </bookViews>
@@ -34,9 +34,147 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>DocEntry</t>
+  </si>
+  <si>
+    <t>123729</t>
+  </si>
+  <si>
+    <t>154974</t>
+  </si>
+  <si>
+    <t>65891</t>
+  </si>
+  <si>
+    <t>114164</t>
+  </si>
+  <si>
+    <t>152122</t>
+  </si>
+  <si>
+    <t>151116</t>
+  </si>
+  <si>
+    <t>102190</t>
+  </si>
+  <si>
+    <t>114446</t>
+  </si>
+  <si>
+    <t>117997</t>
+  </si>
+  <si>
+    <t>147340</t>
+  </si>
+  <si>
+    <t>98679</t>
+  </si>
+  <si>
+    <t>103452</t>
+  </si>
+  <si>
+    <t>93505</t>
+  </si>
+  <si>
+    <t>120498</t>
+  </si>
+  <si>
+    <t>112719</t>
+  </si>
+  <si>
+    <t>93653</t>
+  </si>
+  <si>
+    <t>119106</t>
+  </si>
+  <si>
+    <t>147336</t>
+  </si>
+  <si>
+    <t>108080</t>
+  </si>
+  <si>
+    <t>101189</t>
+  </si>
+  <si>
+    <t>108308</t>
+  </si>
+  <si>
+    <t>101298</t>
+  </si>
+  <si>
+    <t>147322</t>
+  </si>
+  <si>
+    <t>101284</t>
+  </si>
+  <si>
+    <t>101287</t>
+  </si>
+  <si>
+    <t>93654</t>
+  </si>
+  <si>
+    <t>101288</t>
+  </si>
+  <si>
+    <t>101274</t>
+  </si>
+  <si>
+    <t>101276</t>
+  </si>
+  <si>
+    <t>101279</t>
+  </si>
+  <si>
+    <t>152669</t>
+  </si>
+  <si>
+    <t>143647</t>
+  </si>
+  <si>
+    <t>154190</t>
+  </si>
+  <si>
+    <t>101745</t>
+  </si>
+  <si>
+    <t>109324</t>
+  </si>
+  <si>
+    <t>104309</t>
+  </si>
+  <si>
+    <t>140120</t>
+  </si>
+  <si>
+    <t>147228</t>
+  </si>
+  <si>
+    <t>156677</t>
+  </si>
+  <si>
+    <t>162039</t>
+  </si>
+  <si>
+    <t>101775</t>
+  </si>
+  <si>
+    <t>142221</t>
+  </si>
+  <si>
+    <t>149041</t>
+  </si>
+  <si>
+    <t>147932</t>
+  </si>
+  <si>
+    <t>157593</t>
+  </si>
+  <si>
+    <t>162505</t>
   </si>
 </sst>
 </file>
@@ -72,8 +210,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1922D5-C29D-42F9-909F-8E809F7BE4E8}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,58 +544,233 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>73749</v>
+      <c r="A2" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>73753</v>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>73763</v>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>73764</v>
+      <c r="A5" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>73771</v>
+      <c r="A6" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>73801</v>
+      <c r="A7" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>73682</v>
+      <c r="A8" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>73688</v>
+      <c r="A9" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>73698</v>
+      <c r="A10" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>73699</v>
+      <c r="A11" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>73733</v>
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>